<commit_message>
review 2 part 7
</commit_message>
<xml_diff>
--- a/review_2_weather/weather_data_HU.xlsx
+++ b/review_2_weather/weather_data_HU.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,76 +468,64 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:11</t>
+          <t>2023-11-07 17:01:09</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2023-11-07 16:08:18</t>
+          <t>2023-11-07 16:54:38</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sopron</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>10.88</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1.81</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>139</t>
-        </is>
+          <t>Budapest</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>11.09</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:11</t>
+          <t>2023-11-07 17:01:09</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2023-11-07 16:05:49</t>
+          <t>2023-11-07 16:55:16</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Budapest</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>11.57</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1.03</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+          <t>Debrecen</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:11</t>
+          <t>2023-11-07 17:01:09</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2023-11-07 16:06:01</t>
+          <t>2023-11-07 16:56:55</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -545,63 +533,51 @@
           <t>Pécs</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12.98</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1.54</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
+      <c r="D4" t="n">
+        <v>11.98</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:11</t>
+          <t>2023-11-07 17:01:09</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2023-11-07 16:03:49</t>
+          <t>2023-11-07 16:55:24</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Debrecen</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>13.87</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1.03</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Sopron</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>9.33</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="F5" t="n">
+        <v>133</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:11</t>
+          <t>2023-11-07 17:01:09</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2023-11-07 16:07:42</t>
+          <t>2023-11-07 16:57:16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -609,191 +585,155 @@
           <t>Kecskemét</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>14.68</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1.03</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D6" t="n">
+        <v>14.25</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>local timestamp</t>
+          <t>2023-11-07 17:01:49</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>server timestamp</t>
+          <t>2023-11-07 16:59:09</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>city</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>temp</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>wind_speed</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>wind_dir</t>
-        </is>
+          <t>Pécs</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>11.98</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:40</t>
+          <t>2023-11-07 17:01:49</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2023-11-07 16:07:38</t>
+          <t>2023-11-07 16:58:04</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sopron</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>10.88</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1.81</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>139</t>
-        </is>
+          <t>Budapest</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>11.09</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:40</t>
+          <t>2023-11-07 17:01:49</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2023-11-07 16:06:42</t>
+          <t>2023-11-07 17:00:15</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Pécs</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12.98</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1.54</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>260</t>
-        </is>
+          <t>Kecskemét</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>13.28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:40</t>
+          <t>2023-11-07 17:01:49</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2023-11-07 16:06:58</t>
+          <t>2023-11-07 17:00:00</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Debrecen</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>13.87</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1.03</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Sopron</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>9.33</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="F10" t="n">
+        <v>133</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:40</t>
+          <t>2023-11-07 17:01:49</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2023-11-07 16:06:23</t>
+          <t>2023-11-07 17:01:49</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Budapest</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>11.57</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1.03</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+          <t>Debrecen</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2023-11-07 16:14:40</t>
+          <t>2023-11-07 17:02:01</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2023-11-07 16:06:01</t>
+          <t>2023-11-07 17:00:09</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -801,20 +741,118 @@
           <t>Kecskemét</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>15.27</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>1.03</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="D12" t="n">
+        <v>13.33</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-11-07 17:02:01</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2023-11-07 16:59:51</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Budapest</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>11.09</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-11-07 17:02:01</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2023-11-07 16:57:44</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Debrecen</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>12.87</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-11-07 17:02:01</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2023-11-07 17:02:01</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sopron</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>9.02</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="F15" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-11-07 17:02:01</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2023-11-07 17:02:01</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Pécs</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>11.98</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>